<commit_message>
ref 2 was reporoduced by expdata_fit_sci.py
</commit_message>
<xml_diff>
--- a/sample_data/0_reactiondata.xlsx
+++ b/sample_data/0_reactiondata.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mt_oh\DataScience\rxnfit\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721BAD7C-0021-4DE2-B11A-767C386EEE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09F66C0-2A96-447E-97F4-0CE4B3F1C4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F615A3B4-753B-4DCF-9C18-1504BC5FB21C}"/>
   </bookViews>
   <sheets>
     <sheet name="bib2" sheetId="7" r:id="rId1"/>
-    <sheet name="bib3" sheetId="4" r:id="rId2"/>
-    <sheet name="sample_rxn_3" sheetId="5" r:id="rId3"/>
-    <sheet name="sample_timecourse_3" sheetId="6" r:id="rId4"/>
-    <sheet name="bib4" sheetId="2" r:id="rId5"/>
-    <sheet name="sample_rxn_4" sheetId="1" r:id="rId6"/>
-    <sheet name="sample_timecourse_4" sheetId="3" r:id="rId7"/>
+    <sheet name="sample_rxn_2" sheetId="8" r:id="rId2"/>
+    <sheet name="sample_timecourse_2" sheetId="9" r:id="rId3"/>
+    <sheet name="bib3" sheetId="4" r:id="rId4"/>
+    <sheet name="sample_rxn_3" sheetId="5" r:id="rId5"/>
+    <sheet name="sample_timecourse_3" sheetId="6" r:id="rId6"/>
+    <sheet name="bib4" sheetId="2" r:id="rId7"/>
+    <sheet name="sample_rxn_4" sheetId="1" r:id="rId8"/>
+    <sheet name="sample_timecourse_4" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="34">
   <si>
     <t>RID</t>
     <phoneticPr fontId="1"/>
@@ -141,20 +143,79 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>acid_conc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>time_min</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>https://www.nms.ac.jp/library/college/pdf/kenkyujoho/katsudo/kiyou/no44/44thebulletin_takashi_nagai.pdf</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Table 4</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AcOEt</t>
+  </si>
+  <si>
+    <t>AcOEt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>AcOH</t>
+  </si>
+  <si>
+    <t>AcOH</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>EtOH</t>
+  </si>
+  <si>
+    <t>EtOH</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mol/L</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>c[HCl]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>c[acid]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>酢酸濃度は、酸濃度から塩酸濃度を引いたもの</t>
+    <rPh sb="0" eb="2">
+      <t>サクサン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ノウド</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>サン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ノウド</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>エンサン</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ノウド</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ヒ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>&gt;</t>
   </si>
 </sst>
 </file>
@@ -557,205 +618,510 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D901D6-AD11-4C7B-A251-EABA7D7CAD05}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2">
+        <v>0.91620000000000001</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.55779999999999996</v>
+      </c>
+      <c r="C4">
+        <v>51.63</v>
+      </c>
+      <c r="D4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5">
         <v>5.13</v>
       </c>
-      <c r="B4">
+      <c r="B5">
+        <v>0.52569999999999995</v>
+      </c>
+      <c r="C5">
+        <v>51.597900000000003</v>
+      </c>
+      <c r="D5">
+        <v>3.2100000000000017E-2</v>
+      </c>
+      <c r="E5">
+        <v>3.2100000000000017E-2</v>
+      </c>
+      <c r="G5">
         <v>0.94830000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6">
         <v>12.95</v>
       </c>
-      <c r="B5">
+      <c r="B6">
+        <v>0.50629999999999997</v>
+      </c>
+      <c r="C6">
+        <v>51.578500000000005</v>
+      </c>
+      <c r="D6">
+        <v>5.149999999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>5.149999999999999E-2</v>
+      </c>
+      <c r="G6">
         <v>0.9677</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7">
         <v>18.149999999999999</v>
       </c>
-      <c r="B6">
+      <c r="B7">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C7">
+        <v>51.553200000000004</v>
+      </c>
+      <c r="D7">
+        <v>7.6799999999999979E-2</v>
+      </c>
+      <c r="E7">
+        <v>7.6799999999999979E-2</v>
+      </c>
+      <c r="G7">
         <v>0.99299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8">
         <v>29.08</v>
       </c>
-      <c r="B7">
+      <c r="B8">
+        <v>0.45300000000000007</v>
+      </c>
+      <c r="C8">
+        <v>51.525200000000005</v>
+      </c>
+      <c r="D8">
+        <v>0.10479999999999989</v>
+      </c>
+      <c r="E8">
+        <v>0.10479999999999989</v>
+      </c>
+      <c r="G8">
         <v>1.0209999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9">
         <v>40.18</v>
       </c>
-      <c r="B8">
+      <c r="B9">
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="C9">
+        <v>51.497199999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.13279999999999992</v>
+      </c>
+      <c r="E9">
+        <v>0.13279999999999992</v>
+      </c>
+      <c r="G9">
         <v>1.0489999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10">
         <v>51.15</v>
       </c>
-      <c r="B9">
+      <c r="B10">
+        <v>0.39399999999999991</v>
+      </c>
+      <c r="C10">
+        <v>51.466200000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.16380000000000006</v>
+      </c>
+      <c r="E10">
+        <v>0.16380000000000006</v>
+      </c>
+      <c r="G10">
         <v>1.08</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11">
         <v>61.7</v>
       </c>
-      <c r="B10">
+      <c r="B11">
+        <v>0.37399999999999989</v>
+      </c>
+      <c r="C11">
+        <v>51.446200000000005</v>
+      </c>
+      <c r="D11">
+        <v>0.18380000000000007</v>
+      </c>
+      <c r="E11">
+        <v>0.18380000000000007</v>
+      </c>
+      <c r="G11">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12">
         <v>74.75</v>
       </c>
-      <c r="B11">
+      <c r="B12">
+        <v>0.34099999999999997</v>
+      </c>
+      <c r="C12">
+        <v>51.413200000000003</v>
+      </c>
+      <c r="D12">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="G12">
         <v>1.133</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13">
         <v>91.33</v>
       </c>
-      <c r="B12">
+      <c r="B13">
+        <v>0.30499999999999994</v>
+      </c>
+      <c r="C13">
+        <v>51.377200000000002</v>
+      </c>
+      <c r="D13">
+        <v>0.25280000000000002</v>
+      </c>
+      <c r="E13">
+        <v>0.25280000000000002</v>
+      </c>
+      <c r="G13">
         <v>1.169</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14">
         <v>106.58</v>
       </c>
-      <c r="B13">
+      <c r="B14">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C14">
+        <v>51.352200000000003</v>
+      </c>
+      <c r="D14">
+        <v>0.27779999999999994</v>
+      </c>
+      <c r="E14">
+        <v>0.27779999999999994</v>
+      </c>
+      <c r="G14">
         <v>1.194</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15">
         <v>127.57</v>
       </c>
-      <c r="B14">
+      <c r="B15">
+        <v>0.246</v>
+      </c>
+      <c r="C15">
+        <v>51.318200000000004</v>
+      </c>
+      <c r="D15">
+        <v>0.31179999999999997</v>
+      </c>
+      <c r="E15">
+        <v>0.31179999999999997</v>
+      </c>
+      <c r="G15">
         <v>1.228</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16">
         <v>147.88</v>
       </c>
-      <c r="B15">
+      <c r="B16">
+        <v>0.21799999999999997</v>
+      </c>
+      <c r="C16">
+        <v>51.290200000000006</v>
+      </c>
+      <c r="D16">
+        <v>0.33979999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.33979999999999999</v>
+      </c>
+      <c r="G16">
         <v>1.256</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17">
         <v>181</v>
       </c>
-      <c r="B16">
+      <c r="B17">
+        <v>0.17799999999999994</v>
+      </c>
+      <c r="C17">
+        <v>51.2502</v>
+      </c>
+      <c r="D17">
+        <v>0.37980000000000003</v>
+      </c>
+      <c r="E17">
+        <v>0.37980000000000003</v>
+      </c>
+      <c r="G17">
         <v>1.296</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18">
         <v>210.7</v>
       </c>
-      <c r="B17">
+      <c r="B18">
+        <v>0.15300000000000002</v>
+      </c>
+      <c r="C18">
+        <v>51.225200000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.40479999999999994</v>
+      </c>
+      <c r="E18">
+        <v>0.40479999999999994</v>
+      </c>
+      <c r="G18">
         <v>1.321</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19">
         <v>240.85</v>
       </c>
-      <c r="B18">
+      <c r="B19">
+        <v>0.127</v>
+      </c>
+      <c r="C19">
+        <v>51.199200000000005</v>
+      </c>
+      <c r="D19">
+        <v>0.43079999999999996</v>
+      </c>
+      <c r="E19">
+        <v>0.43079999999999996</v>
+      </c>
+      <c r="G19">
         <v>1.347</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20">
         <v>300.72000000000003</v>
       </c>
-      <c r="B19">
+      <c r="B20">
+        <v>0.10099999999999998</v>
+      </c>
+      <c r="C20">
+        <v>51.173200000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.45679999999999998</v>
+      </c>
+      <c r="E20">
+        <v>0.45679999999999998</v>
+      </c>
+      <c r="G20">
         <v>1.373</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21">
         <v>367.65</v>
       </c>
-      <c r="B20">
+      <c r="B21">
+        <v>7.4000000000000066E-2</v>
+      </c>
+      <c r="C21">
+        <v>51.1462</v>
+      </c>
+      <c r="D21">
+        <v>0.4837999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0.4837999999999999</v>
+      </c>
+      <c r="G21">
         <v>1.4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22">
         <v>420.97</v>
       </c>
-      <c r="B21">
+      <c r="B22">
+        <v>5.8000000000000052E-2</v>
+      </c>
+      <c r="C22">
+        <v>51.130200000000002</v>
+      </c>
+      <c r="D22">
+        <v>0.49979999999999991</v>
+      </c>
+      <c r="E22">
+        <v>0.49979999999999991</v>
+      </c>
+      <c r="G22">
         <v>1.4159999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23">
         <v>486.52</v>
       </c>
-      <c r="B22">
+      <c r="B23">
+        <v>5.0999999999999934E-2</v>
+      </c>
+      <c r="C23">
+        <v>51.123200000000004</v>
+      </c>
+      <c r="D23">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="E23">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="G23">
         <v>1.423</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24">
         <v>555.48</v>
       </c>
-      <c r="B23">
+      <c r="B24">
+        <v>4.0999999999999925E-2</v>
+      </c>
+      <c r="C24">
+        <v>51.113199999999999</v>
+      </c>
+      <c r="D24">
+        <v>0.51680000000000004</v>
+      </c>
+      <c r="E24">
+        <v>0.51680000000000004</v>
+      </c>
+      <c r="G24">
         <v>1.4330000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25">
         <v>1569.3</v>
       </c>
-      <c r="B24">
+      <c r="B25">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="C25">
+        <v>51.102200000000003</v>
+      </c>
+      <c r="D25">
+        <v>0.52779999999999994</v>
+      </c>
+      <c r="E25">
+        <v>0.52779999999999994</v>
+      </c>
+      <c r="G25">
         <v>1.444</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26">
         <v>1712.15</v>
       </c>
-      <c r="B25">
+      <c r="B26">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="C26">
+        <v>51.102200000000003</v>
+      </c>
+      <c r="D26">
+        <v>0.52779999999999994</v>
+      </c>
+      <c r="E26">
+        <v>0.52779999999999994</v>
+      </c>
+      <c r="G26">
         <v>1.444</v>
       </c>
     </row>
@@ -769,11 +1135,533 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079CB5AB-A81E-499F-86D9-334B10A5669A}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1.2300000000000001E-4</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>7.0899999999999999E-4</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6187E9E3-D486-41BA-9579-F990B4AF2F51}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.55779999999999996</v>
+      </c>
+      <c r="C2">
+        <v>51.63</v>
+      </c>
+      <c r="D2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>5.13</v>
+      </c>
+      <c r="B3">
+        <v>0.52569999999999995</v>
+      </c>
+      <c r="C3">
+        <v>51.597900000000003</v>
+      </c>
+      <c r="D3">
+        <v>3.2100000000000017E-2</v>
+      </c>
+      <c r="E3">
+        <v>3.2100000000000017E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>12.95</v>
+      </c>
+      <c r="B4">
+        <v>0.50629999999999997</v>
+      </c>
+      <c r="C4">
+        <v>51.578500000000005</v>
+      </c>
+      <c r="D4">
+        <v>5.149999999999999E-2</v>
+      </c>
+      <c r="E4">
+        <v>5.149999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>18.149999999999999</v>
+      </c>
+      <c r="B5">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C5">
+        <v>51.553200000000004</v>
+      </c>
+      <c r="D5">
+        <v>7.6799999999999979E-2</v>
+      </c>
+      <c r="E5">
+        <v>7.6799999999999979E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>29.08</v>
+      </c>
+      <c r="B6">
+        <v>0.45300000000000007</v>
+      </c>
+      <c r="C6">
+        <v>51.525200000000005</v>
+      </c>
+      <c r="D6">
+        <v>0.10479999999999989</v>
+      </c>
+      <c r="E6">
+        <v>0.10479999999999989</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>40.18</v>
+      </c>
+      <c r="B7">
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="C7">
+        <v>51.497199999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.13279999999999992</v>
+      </c>
+      <c r="E7">
+        <v>0.13279999999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>51.15</v>
+      </c>
+      <c r="B8">
+        <v>0.39399999999999991</v>
+      </c>
+      <c r="C8">
+        <v>51.466200000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.16380000000000006</v>
+      </c>
+      <c r="E8">
+        <v>0.16380000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>61.7</v>
+      </c>
+      <c r="B9">
+        <v>0.37399999999999989</v>
+      </c>
+      <c r="C9">
+        <v>51.446200000000005</v>
+      </c>
+      <c r="D9">
+        <v>0.18380000000000007</v>
+      </c>
+      <c r="E9">
+        <v>0.18380000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>74.75</v>
+      </c>
+      <c r="B10">
+        <v>0.34099999999999997</v>
+      </c>
+      <c r="C10">
+        <v>51.413200000000003</v>
+      </c>
+      <c r="D10">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0.21679999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>91.33</v>
+      </c>
+      <c r="B11">
+        <v>0.30499999999999994</v>
+      </c>
+      <c r="C11">
+        <v>51.377200000000002</v>
+      </c>
+      <c r="D11">
+        <v>0.25280000000000002</v>
+      </c>
+      <c r="E11">
+        <v>0.25280000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>106.58</v>
+      </c>
+      <c r="B12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C12">
+        <v>51.352200000000003</v>
+      </c>
+      <c r="D12">
+        <v>0.27779999999999994</v>
+      </c>
+      <c r="E12">
+        <v>0.27779999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>127.57</v>
+      </c>
+      <c r="B13">
+        <v>0.246</v>
+      </c>
+      <c r="C13">
+        <v>51.318200000000004</v>
+      </c>
+      <c r="D13">
+        <v>0.31179999999999997</v>
+      </c>
+      <c r="E13">
+        <v>0.31179999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>147.88</v>
+      </c>
+      <c r="B14">
+        <v>0.21799999999999997</v>
+      </c>
+      <c r="C14">
+        <v>51.290200000000006</v>
+      </c>
+      <c r="D14">
+        <v>0.33979999999999999</v>
+      </c>
+      <c r="E14">
+        <v>0.33979999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>181</v>
+      </c>
+      <c r="B15">
+        <v>0.17799999999999994</v>
+      </c>
+      <c r="C15">
+        <v>51.2502</v>
+      </c>
+      <c r="D15">
+        <v>0.37980000000000003</v>
+      </c>
+      <c r="E15">
+        <v>0.37980000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>210.7</v>
+      </c>
+      <c r="B16">
+        <v>0.15300000000000002</v>
+      </c>
+      <c r="C16">
+        <v>51.225200000000001</v>
+      </c>
+      <c r="D16">
+        <v>0.40479999999999994</v>
+      </c>
+      <c r="E16">
+        <v>0.40479999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>240.85</v>
+      </c>
+      <c r="B17">
+        <v>0.127</v>
+      </c>
+      <c r="C17">
+        <v>51.199200000000005</v>
+      </c>
+      <c r="D17">
+        <v>0.43079999999999996</v>
+      </c>
+      <c r="E17">
+        <v>0.43079999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>300.72000000000003</v>
+      </c>
+      <c r="B18">
+        <v>0.10099999999999998</v>
+      </c>
+      <c r="C18">
+        <v>51.173200000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.45679999999999998</v>
+      </c>
+      <c r="E18">
+        <v>0.45679999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>367.65</v>
+      </c>
+      <c r="B19">
+        <v>7.4000000000000066E-2</v>
+      </c>
+      <c r="C19">
+        <v>51.1462</v>
+      </c>
+      <c r="D19">
+        <v>0.4837999999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.4837999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>420.97</v>
+      </c>
+      <c r="B20">
+        <v>5.8000000000000052E-2</v>
+      </c>
+      <c r="C20">
+        <v>51.130200000000002</v>
+      </c>
+      <c r="D20">
+        <v>0.49979999999999991</v>
+      </c>
+      <c r="E20">
+        <v>0.49979999999999991</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>486.52</v>
+      </c>
+      <c r="B21">
+        <v>5.0999999999999934E-2</v>
+      </c>
+      <c r="C21">
+        <v>51.123200000000004</v>
+      </c>
+      <c r="D21">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="E21">
+        <v>0.50680000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>555.48</v>
+      </c>
+      <c r="B22">
+        <v>4.0999999999999925E-2</v>
+      </c>
+      <c r="C22">
+        <v>51.113199999999999</v>
+      </c>
+      <c r="D22">
+        <v>0.51680000000000004</v>
+      </c>
+      <c r="E22">
+        <v>0.51680000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>1569.3</v>
+      </c>
+      <c r="B23">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="C23">
+        <v>51.102200000000003</v>
+      </c>
+      <c r="D23">
+        <v>0.52779999999999994</v>
+      </c>
+      <c r="E23">
+        <v>0.52779999999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>1712.15</v>
+      </c>
+      <c r="B24">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="C24">
+        <v>51.102200000000003</v>
+      </c>
+      <c r="D24">
+        <v>0.52779999999999994</v>
+      </c>
+      <c r="E24">
+        <v>0.52779999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D208C04-369C-4879-9957-78E3E3AB5306}">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -801,7 +1689,7 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>1.15E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -833,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>1.18E-2</v>
+        <v>0.191</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -1112,11 +2000,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0C9A00-04EB-42C5-AFB3-407899577BF6}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -1133,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.15E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -1218,11 +2108,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD8B6F3-70C3-4EB5-B176-95867C52FCBA}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -1431,7 +2323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43A8467-E8F3-4BAC-B190-82BFA025ED00}">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -1608,7 +2500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{560F0BA0-3013-4C3F-B4B1-EFC293A03671}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1683,7 +2575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7CCEFD-693B-4C58-B579-44C45EF10570}">
   <dimension ref="A1:D6"/>
   <sheetViews>

</xml_diff>